<commit_message>
Updated the xlsx file, seemed to be causing a data error with the one currently on the site
</commit_message>
<xml_diff>
--- a/dash/assets/GLEON_GMA_Example.xlsx
+++ b/dash/assets/GLEON_GMA_Example.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saba/GLEON-GMA/dash/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9ED398-AAE2-574B-9995-602628D29BF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14020"/>
   </bookViews>
   <sheets>
     <sheet name="GLEON_GMA_Example csv" sheetId="1" r:id="rId1"/>
     <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -407,8 +406,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1026,7 +1025,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1062,6 +1061,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1163,7 +1164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1215,7 +1216,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1409,25 +1410,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
@@ -1438,7 +1439,7 @@
     <col min="14" max="14" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.83203125" style="16" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14.83203125" customWidth="1"/>
     <col min="48" max="48" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="17.1640625" bestFit="1" customWidth="1"/>
@@ -1543,7 +1544,7 @@
       <c r="AE1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="15" t="s">
         <v>33</v>
       </c>
       <c r="AG1" s="2" t="s">
@@ -1615,25 +1616,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="72.6640625" customWidth="1"/>
     <col min="3" max="3" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1">
+    <row r="1" spans="1:3" ht="15" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -1644,7 +1650,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+    <row r="2" spans="1:3" ht="15" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>126</v>
       </c>
@@ -1655,7 +1661,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1">
+    <row r="3" spans="1:3" ht="15" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1">
+    <row r="4" spans="1:3" ht="15" thickBot="1">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1">
+    <row r="5" spans="1:3" ht="15" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>106</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1">
+    <row r="6" spans="1:3" ht="15" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>60</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1">
+    <row r="7" spans="1:3" ht="15" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1">
+    <row r="8" spans="1:3" ht="15" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1">
+    <row r="9" spans="1:3" ht="15" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1">
+    <row r="10" spans="1:3" ht="15" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" thickBot="1">
+    <row r="11" spans="1:3" ht="15" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+    <row r="12" spans="1:3" ht="15" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1">
+    <row r="13" spans="1:3" ht="15" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29" thickBot="1">
+    <row r="14" spans="1:3" ht="25" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" thickBot="1">
+    <row r="15" spans="1:3" ht="15" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1">
+    <row r="16" spans="1:3" ht="15" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" thickBot="1">
+    <row r="17" spans="1:3" ht="15" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1">
+    <row r="18" spans="1:3" ht="15" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>16</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" thickBot="1">
+    <row r="19" spans="1:3" ht="15" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1">
+    <row r="20" spans="1:3" ht="15" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" thickBot="1">
+    <row r="21" spans="1:3" ht="15" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>20</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" thickBot="1">
+    <row r="22" spans="1:3" ht="15" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>21</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" thickBot="1">
+    <row r="23" spans="1:3" ht="15" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>22</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" thickBot="1">
+    <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>23</v>
       </c>
@@ -1897,7 +1903,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" thickBot="1">
+    <row r="25" spans="1:3" ht="15" thickBot="1">
       <c r="A25" s="9" t="s">
         <v>24</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" thickBot="1">
+    <row r="26" spans="1:3" ht="15" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>25</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" thickBot="1">
+    <row r="27" spans="1:3" ht="15" thickBot="1">
       <c r="A27" s="9" t="s">
         <v>26</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" thickBot="1">
+    <row r="28" spans="1:3" ht="15" thickBot="1">
       <c r="A28" s="9" t="s">
         <v>27</v>
       </c>
@@ -1941,7 +1947,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" thickBot="1">
+    <row r="29" spans="1:3" ht="15" thickBot="1">
       <c r="A29" s="9" t="s">
         <v>28</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" thickBot="1">
+    <row r="30" spans="1:3" ht="15" thickBot="1">
       <c r="A30" s="9" t="s">
         <v>29</v>
       </c>
@@ -1963,7 +1969,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" thickBot="1">
+    <row r="31" spans="1:3" ht="15" thickBot="1">
       <c r="A31" s="9" t="s">
         <v>30</v>
       </c>
@@ -1974,7 +1980,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" thickBot="1">
+    <row r="32" spans="1:3" ht="15" thickBot="1">
       <c r="A32" s="9" t="s">
         <v>31</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" thickBot="1">
+    <row r="33" spans="1:3" ht="15" thickBot="1">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" thickBot="1">
+    <row r="34" spans="1:3" ht="15" thickBot="1">
       <c r="A34" s="9" t="s">
         <v>110</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" thickBot="1">
+    <row r="35" spans="1:3" ht="15" thickBot="1">
       <c r="A35" s="9" t="s">
         <v>124</v>
       </c>
@@ -2018,7 +2024,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" thickBot="1">
+    <row r="36" spans="1:3" ht="15" thickBot="1">
       <c r="A36" s="9" t="s">
         <v>36</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" thickBot="1">
+    <row r="37" spans="1:3" ht="15" thickBot="1">
       <c r="A37" s="9" t="s">
         <v>35</v>
       </c>
@@ -2040,7 +2046,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" thickBot="1">
+    <row r="38" spans="1:3" ht="15" thickBot="1">
       <c r="A38" s="9" t="s">
         <v>34</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" thickBot="1">
+    <row r="39" spans="1:3" ht="15" thickBot="1">
       <c r="A39" s="9" t="s">
         <v>37</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" thickBot="1">
+    <row r="40" spans="1:3" ht="15" thickBot="1">
       <c r="A40" s="9" t="s">
         <v>38</v>
       </c>
@@ -2073,7 +2079,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" thickBot="1">
+    <row r="41" spans="1:3" ht="15" thickBot="1">
       <c r="A41" s="9" t="s">
         <v>39</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" thickBot="1">
+    <row r="42" spans="1:3" ht="15" thickBot="1">
       <c r="A42" s="9" t="s">
         <v>40</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" thickBot="1">
+    <row r="43" spans="1:3" ht="15" thickBot="1">
       <c r="A43" s="9" t="s">
         <v>41</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" thickBot="1">
+    <row r="44" spans="1:3" ht="15" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>42</v>
       </c>
@@ -2117,7 +2123,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" thickBot="1">
+    <row r="45" spans="1:3" ht="15" thickBot="1">
       <c r="A45" s="9" t="s">
         <v>43</v>
       </c>
@@ -2128,7 +2134,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" thickBot="1">
+    <row r="46" spans="1:3" ht="15" thickBot="1">
       <c r="A46" s="11" t="s">
         <v>44</v>
       </c>
@@ -2229,5 +2235,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>